<commit_message>
Commiting documents for scrum flavor
</commit_message>
<xml_diff>
--- a/Team Metric Charts.xlsx
+++ b/Team Metric Charts.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Experian\Sprint-Review Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Experian\Sprint-Review Docs\agile-scrum-documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="96" windowWidth="17760" windowHeight="7308" tabRatio="745" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="96" windowWidth="17760" windowHeight="7308" tabRatio="745"/>
   </bookViews>
   <sheets>
-    <sheet name="Goblins Release Burn-up" sheetId="5" r:id="rId1"/>
-    <sheet name="Goblins Velocity" sheetId="4" r:id="rId2"/>
-    <sheet name="Goblins Focus Factor" sheetId="8" r:id="rId3"/>
+    <sheet name="Team Release Burn-up" sheetId="5" r:id="rId1"/>
+    <sheet name="Team Velocity" sheetId="4" r:id="rId2"/>
+    <sheet name="Team Focus Factor" sheetId="8" r:id="rId3"/>
     <sheet name="Quality Gates" sheetId="11" r:id="rId4"/>
     <sheet name="Sheet1" sheetId="25" r:id="rId5"/>
   </sheets>
@@ -121,9 +121,6 @@
     <t>Rhea</t>
   </si>
   <si>
-    <t>2018R1 - Originations Bugs Trend (end of each sprint)</t>
-  </si>
-  <si>
     <t>2018R1 - Originations Veracode Medium Flaws Trend</t>
   </si>
   <si>
@@ -146,6 +143,9 @@
   </si>
   <si>
     <t>Sprint 21</t>
+  </si>
+  <si>
+    <t>2018R1 - Product Bugs Trend (end of each sprint)</t>
   </si>
 </sst>
 </file>
@@ -296,7 +296,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Goblins 2018R1 </a:t>
+              <a:t>Team 2018R1 </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
@@ -330,7 +330,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Goblins Release Burn-up'!$C$3</c:f>
+              <c:f>'Team Release Burn-up'!$C$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -374,7 +374,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Goblins Release Burn-up'!$B$4:$B$13</c:f>
+              <c:f>'Team Release Burn-up'!$B$4:$B$13</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -412,7 +412,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Goblins Release Burn-up'!$C$4:$C$13</c:f>
+              <c:f>'Team Release Burn-up'!$C$4:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -451,7 +451,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Goblins Release Burn-up'!$D$3</c:f>
+              <c:f>'Team Release Burn-up'!$D$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -508,7 +508,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Goblins Release Burn-up'!$B$4:$B$13</c:f>
+              <c:f>'Team Release Burn-up'!$B$4:$B$13</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -546,7 +546,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Goblins Release Burn-up'!$D$4:$D$13</c:f>
+              <c:f>'Team Release Burn-up'!$D$4:$D$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -601,7 +601,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Goblins Release Burn-up'!$E$3</c:f>
+              <c:f>'Team Release Burn-up'!$E$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -633,7 +633,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Goblins Release Burn-up'!$B$4:$B$13</c:f>
+              <c:f>'Team Release Burn-up'!$B$4:$B$13</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -671,7 +671,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Goblins Release Burn-up'!$E$4:$E$13</c:f>
+              <c:f>'Team Release Burn-up'!$E$4:$E$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -827,7 +827,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Goblins 2018R1 Sprint Velocity &amp; Average Velocity</a:t>
+              <a:t>Team 2018R1 Sprint Velocity &amp; Average Velocity</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -903,7 +903,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Goblins Velocity'!$B$4:$B$24</c:f>
+              <c:f>'Team Velocity'!$B$4:$B$24</c:f>
               <c:strCache>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
@@ -974,7 +974,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Goblins Velocity'!$C$4:$C$24</c:f>
+              <c:f>'Team Velocity'!$C$4:$C$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -1056,7 +1056,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Goblins Velocity'!$B$4:$B$24</c:f>
+              <c:f>'Team Velocity'!$B$4:$B$24</c:f>
               <c:strCache>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
@@ -1127,7 +1127,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Goblins Velocity'!$D$4:$D$24</c:f>
+              <c:f>'Team Velocity'!$D$4:$D$24</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="21"/>
@@ -1314,7 +1314,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Goblins Focus Factor</a:t>
+              <a:t>Team Focus Factor</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1332,7 +1332,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Goblins Focus Factor'!$E$3</c:f>
+              <c:f>'Team Focus Factor'!$E$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1368,7 +1368,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Goblins Focus Factor'!$B$4:$B$24</c:f>
+              <c:f>'Team Focus Factor'!$B$4:$B$24</c:f>
               <c:strCache>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
@@ -1439,7 +1439,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Goblins Focus Factor'!$E$4:$E$24</c:f>
+              <c:f>'Team Focus Factor'!$E$4:$E$24</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="21"/>
@@ -1623,7 +1623,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Originations </a:t>
+              <a:t>Product </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
@@ -3445,8 +3445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:I18"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3663,8 +3663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P34" sqref="P34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3864,7 +3864,7 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C18">
         <v>98</v>
@@ -3875,7 +3875,7 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C19">
         <v>77</v>
@@ -3886,7 +3886,7 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20">
         <v>111</v>
@@ -3897,7 +3897,7 @@
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C21">
         <v>117</v>
@@ -3908,7 +3908,7 @@
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C22">
         <v>47</v>
@@ -3919,7 +3919,7 @@
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C23">
         <v>104</v>
@@ -3930,7 +3930,7 @@
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C24">
         <v>105</v>
@@ -3950,8 +3950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:E25"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="S26" sqref="S26"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4183,7 +4183,7 @@
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C18">
         <v>95</v>
@@ -4198,7 +4198,7 @@
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C19">
         <v>75</v>
@@ -4213,7 +4213,7 @@
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20">
         <v>100</v>
@@ -4228,7 +4228,7 @@
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C21">
         <v>100</v>
@@ -4243,7 +4243,7 @@
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C22">
         <v>47</v>
@@ -4258,7 +4258,7 @@
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C23">
         <v>95</v>
@@ -4273,7 +4273,7 @@
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C24">
         <v>95</v>
@@ -4310,7 +4310,7 @@
   <dimension ref="A1:H94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A84" sqref="A84:G96"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4329,7 +4329,7 @@
     </row>
     <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="10" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -4473,7 +4473,7 @@
     </row>
     <row r="31" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>